<commit_message>
Incorporate files from UT
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SYDEC/Start Year Distributed Electricity Capacity.xlsx
+++ b/InputData/bldgs/SYDEC/Start Year Distributed Electricity Capacity.xlsx
@@ -3594,13 +3594,13 @@
         <v>15</v>
       </c>
       <c r="B7" s="4">
-        <v>29.474481412656953</v>
+        <v>275.23957626713974</v>
       </c>
       <c r="C7" s="4">
-        <v>10.402758145643634</v>
+        <v>97.143379858990528</v>
       </c>
       <c r="D7" s="4">
-        <v>6.334286539910563</v>
+        <v>59.151043873869753</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" x14ac:dyDescent="0.45">

</xml_diff>